<commit_message>
Edit tasks. Edit styles for page title and for article page. Signed-off-by:Igor Peshkov <igor.peshkov@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/task/tasks.xlsx
+++ b/docs/task/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Number</t>
   </si>
@@ -89,13 +89,19 @@
   <si>
     <t>UserController/InfoAction
 UserController/AllAction</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Создана страница для просмотра пользователей. Выводится по 9 пользователей на страницу.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +144,22 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +184,16 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -285,10 +315,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -335,9 +367,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -362,50 +391,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <font>
-        <i/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -596,6 +594,30 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -629,25 +651,40 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-      </border>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -660,30 +697,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F58" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F58" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:F58"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Number" dataDxfId="3"/>
-    <tableColumn id="2" name="Task" dataDxfId="2"/>
-    <tableColumn id="3" name="Task Location" dataDxfId="0"/>
-    <tableColumn id="6" name="Priority" dataDxfId="1"/>
-    <tableColumn id="4" name="Status" dataDxfId="7"/>
-    <tableColumn id="5" name="Description" dataDxfId="6"/>
+    <tableColumn id="1" name="Number" dataDxfId="16"/>
+    <tableColumn id="2" name="Task" dataDxfId="15"/>
+    <tableColumn id="3" name="Task Location" dataDxfId="14"/>
+    <tableColumn id="6" name="Priority" dataDxfId="13"/>
+    <tableColumn id="4" name="Status" dataDxfId="12"/>
+    <tableColumn id="5" name="Description" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F8" totalsRowShown="0" headerRowDxfId="15" dataDxfId="8" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Number" dataDxfId="14"/>
-    <tableColumn id="2" name="Bug" dataDxfId="13"/>
-    <tableColumn id="3" name="Bug Location" dataDxfId="12"/>
-    <tableColumn id="4" name="Priority" dataDxfId="11"/>
-    <tableColumn id="5" name="Status" dataDxfId="10"/>
-    <tableColumn id="6" name="Description" dataDxfId="9"/>
+    <tableColumn id="1" name="Number" dataDxfId="5"/>
+    <tableColumn id="2" name="Bug" dataDxfId="4"/>
+    <tableColumn id="3" name="Bug Location" dataDxfId="3"/>
+    <tableColumn id="4" name="Priority" dataDxfId="2"/>
+    <tableColumn id="5" name="Status" dataDxfId="1"/>
+    <tableColumn id="6" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -979,7 +1016,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,13 +1056,13 @@
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="27" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1039,13 +1076,13 @@
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="27" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="4"/>
@@ -1057,34 +1094,36 @@
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="27" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="4"/>
+      <c r="E5" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
@@ -1093,13 +1132,13 @@
       <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="27" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4"/>
@@ -1109,7 +1148,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="25"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="4"/>
@@ -1119,7 +1158,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="25"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="4"/>
@@ -1130,7 +1169,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="25"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="4"/>
@@ -1140,7 +1179,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="25"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="4"/>
@@ -1150,7 +1189,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="25"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="4"/>
@@ -1160,7 +1199,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="25"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="4"/>
@@ -1170,7 +1209,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="25"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="4"/>
@@ -1180,7 +1219,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="25"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="4"/>
@@ -1190,7 +1229,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="25"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="4"/>
@@ -1200,7 +1239,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="25"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="4"/>
@@ -1210,7 +1249,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="25"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="4"/>
@@ -1220,7 +1259,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="25"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="4"/>
@@ -1230,7 +1269,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="25"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="4"/>
@@ -1240,7 +1279,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="25"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="4"/>
@@ -1250,7 +1289,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="25"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="4"/>
@@ -1260,7 +1299,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="25"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="4"/>
@@ -1270,7 +1309,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="25"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="4"/>
@@ -1280,7 +1319,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="25"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="4"/>
@@ -1290,7 +1329,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="25"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="4"/>
@@ -1300,7 +1339,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="25"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="4"/>
@@ -1310,7 +1349,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="C27" s="25"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="4"/>
@@ -1320,7 +1359,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4"/>
-      <c r="C28" s="25"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="4"/>
@@ -1330,7 +1369,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="C29" s="25"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="4"/>
@@ -1340,7 +1379,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="25"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="4"/>
@@ -1350,7 +1389,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="25"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="4"/>
@@ -1360,7 +1399,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="25"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="4"/>
@@ -1370,7 +1409,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4"/>
-      <c r="C33" s="25"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="4"/>
@@ -1380,7 +1419,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4"/>
-      <c r="C34" s="25"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="4"/>
@@ -1390,7 +1429,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4"/>
-      <c r="C35" s="25"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="4"/>
@@ -1400,7 +1439,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4"/>
-      <c r="C36" s="25"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="4"/>
@@ -1410,7 +1449,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4"/>
-      <c r="C37" s="25"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="4"/>
@@ -1420,7 +1459,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4"/>
-      <c r="C38" s="25"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="4"/>
@@ -1430,7 +1469,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4"/>
-      <c r="C39" s="25"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="4"/>
@@ -1440,7 +1479,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4"/>
-      <c r="C40" s="25"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="4"/>
@@ -1450,7 +1489,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4"/>
-      <c r="C41" s="25"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="4"/>
@@ -1460,7 +1499,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="4"/>
-      <c r="C42" s="25"/>
+      <c r="C42" s="24"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="4"/>
@@ -1470,7 +1509,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="4"/>
-      <c r="C43" s="25"/>
+      <c r="C43" s="24"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="4"/>
@@ -1480,7 +1519,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4"/>
-      <c r="C44" s="25"/>
+      <c r="C44" s="24"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="4"/>
@@ -1490,7 +1529,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="4"/>
-      <c r="C45" s="25"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="4"/>
@@ -1500,7 +1539,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="4"/>
-      <c r="C46" s="25"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="4"/>
@@ -1510,7 +1549,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4"/>
-      <c r="C47" s="25"/>
+      <c r="C47" s="24"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="4"/>
@@ -1520,7 +1559,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="4"/>
-      <c r="C48" s="25"/>
+      <c r="C48" s="24"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="4"/>
@@ -1530,7 +1569,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="4"/>
-      <c r="C49" s="25"/>
+      <c r="C49" s="24"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="4"/>
@@ -1540,7 +1579,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="4"/>
-      <c r="C50" s="25"/>
+      <c r="C50" s="24"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="4"/>
@@ -1550,7 +1589,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="4"/>
-      <c r="C51" s="25"/>
+      <c r="C51" s="24"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="4"/>
@@ -1560,7 +1599,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="4"/>
-      <c r="C52" s="25"/>
+      <c r="C52" s="24"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="4"/>
@@ -1570,7 +1609,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="4"/>
-      <c r="C53" s="25"/>
+      <c r="C53" s="24"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="4"/>
@@ -1580,7 +1619,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="4"/>
-      <c r="C54" s="25"/>
+      <c r="C54" s="24"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="4"/>
@@ -1590,7 +1629,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="4"/>
-      <c r="C55" s="25"/>
+      <c r="C55" s="24"/>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="4"/>
@@ -1600,7 +1639,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="4"/>
-      <c r="C56" s="25"/>
+      <c r="C56" s="24"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="4"/>
@@ -1610,7 +1649,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="4"/>
-      <c r="C57" s="25"/>
+      <c r="C57" s="24"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="4"/>
@@ -1620,7 +1659,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="4"/>
-      <c r="C58" s="25"/>
+      <c r="C58" s="24"/>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="4"/>
@@ -1672,37 +1711,37 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="13"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="19"/>
+      <c r="E2" s="18"/>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>2</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="7"/>
       <c r="D3" s="17"/>
-      <c r="E3" s="20"/>
+      <c r="E3" s="19"/>
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="13"/>
       <c r="D4" s="15"/>
-      <c r="E4" s="19"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="22">
         <v>4</v>
       </c>
       <c r="B5" s="8"/>
@@ -1712,7 +1751,7 @@
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
       <c r="B6" s="5"/>
@@ -1722,7 +1761,7 @@
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="22">
         <v>6</v>
       </c>
       <c r="B7" s="8"/>
@@ -1732,13 +1771,13 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="24">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="16"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add functional for artcile add, view, all pages. Add translations. Signed-off-by:Igor Peshkov <igor.peshkov@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/task/tasks.xlsx
+++ b/docs/task/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Number</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Forms/UserActivateForm</t>
-  </si>
-  <si>
-    <t>После добавления декораторов глянуть не повлекло ли это изминений в дизайне сайта.</t>
   </si>
   <si>
     <t>Добавить функцию востановление пароля</t>
@@ -95,13 +92,30 @@
   </si>
   <si>
     <t>Создана страница для просмотра пользователей. Выводится по 9 пользователей на страницу.</t>
+  </si>
+  <si>
+    <t>Not fully</t>
+  </si>
+  <si>
+    <t>Придумать общую структуру для всего сайта для кнопок формы.</t>
+  </si>
+  <si>
+    <t>ArctileController/AllAction
+ArctileController/View
+ArctileController/Add</t>
+  </si>
+  <si>
+    <t>По окончанию протестировать права пользователей, которые могут редактировать текст статьи</t>
+  </si>
+  <si>
+    <t>Реализовать функционал добавление статей на сайт, вывод их на главной странице через пейджер по 10 штук на странице, текст статьи выводить в ограниченом виде. Заглавие страницы сделать ссылкой на статью, такой же функционал сделать для кнопки "читать полностью".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,8 +172,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +215,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -315,12 +341,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -397,10 +424,14 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
@@ -1016,7 +1047,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1082,7 @@
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -1062,11 +1093,11 @@
       <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="27" t="s">
-        <v>7</v>
+      <c r="E2" s="28" t="s">
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1074,13 +1105,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>12</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>7</v>
@@ -1092,10 +1123,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>6</v>
@@ -1110,19 +1141,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="D5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>21</v>
-      </c>
       <c r="E5" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1130,28 +1161,38 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
@@ -1695,10 +1736,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Add jQuery carousel for last 10 articles on the main page. Edit chat controller. Add functional for edited and edited articles. Add translations. Add models for Article type and Content type. Updated jQuery UI js and css. Signed-off-by:Igor Peshkov <igor.peshkov@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/task/tasks.xlsx
+++ b/docs/task/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Number</t>
   </si>
@@ -109,13 +109,28 @@
   </si>
   <si>
     <t>Реализовать функционал добавление статей на сайт, вывод их на главной странице через пейджер по 10 штук на странице, текст статьи выводить в ограниченом виде. Заглавие страницы сделать ссылкой на статью, такой же функционал сделать для кнопки "читать полностью".</t>
+  </si>
+  <si>
+    <t>user/edit</t>
+  </si>
+  <si>
+    <t>Когда админ редактирует профиль какого либо пользователя и сохраняет, то результат измения сохранятся в профиль админа.</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Реализоватьфункционал востановление паролья для пользователя. </t>
+  </si>
+  <si>
+    <t>user/restorepasswd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +194,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -347,7 +369,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -425,6 +447,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1047,7 +1075,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,10 +1215,10 @@
       <c r="D7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="29" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1198,10 +1226,18 @@
       <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>7</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="H8" s="4"/>
     </row>
@@ -1719,7 +1755,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,14 +1787,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>7</v>
+      </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add article type, game and mod controler. New design. New jquery, Signed-off-by:Igor Peshkov <igor.peshkov@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/task/tasks.xlsx
+++ b/docs/task/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Number</t>
   </si>
@@ -120,10 +120,28 @@
     <t>Normal</t>
   </si>
   <si>
-    <t xml:space="preserve">Реализоватьфункционал востановление паролья для пользователя. </t>
-  </si>
-  <si>
-    <t>user/restorepasswd</t>
+    <t>ArticleTypeController</t>
+  </si>
+  <si>
+    <t>Добавить кнопки "отмена" на страницы редактирования статей.</t>
+  </si>
+  <si>
+    <t>ArctileController/Edit</t>
+  </si>
+  <si>
+    <t>После нажатия на эту кнопку следует возратить на страницу просмотра статьи</t>
+  </si>
+  <si>
+    <t>Переделать ACL класс. Заменить два запроса достающие сначала номер роли, а потом имя роли на один с джойном.</t>
+  </si>
+  <si>
+    <t>ACL class</t>
+  </si>
+  <si>
+    <t>Mdium</t>
+  </si>
+  <si>
+    <t>Реализовать добавления типов статей через админку в бд. А так же их выбор при создании статьи.</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1093,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,15 +1240,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>34</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>20</v>
@@ -1241,24 +1259,42 @@
       <c r="F8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>7</v>
+      </c>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add new functionality for articles types. Add new FirstBoot controller. Signed-off-by:Igor Peshkov <igor.peshkov@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/task/tasks.xlsx
+++ b/docs/task/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Number</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>Реализовать добавления типов статей через админку в бд. А так же их выбор при создании статьи.</t>
+  </si>
+  <si>
+    <t>Реализовать добавление лиг на сайте. Редатирование, удаление.</t>
+  </si>
+  <si>
+    <t>LeagueController 
+Add
+Edit
+Delete</t>
+  </si>
+  <si>
+    <t>Статьи править и просматривать может только мастер. Админ может только просматривать.</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1105,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,10 +1265,12 @@
       <c r="D8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4"/>
+      <c r="E8" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1297,14 +1311,22 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+      <c r="B11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>7</v>
+      </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add some functionality for Game controller. Signed-off-by:Igor Peshkov <igor.peshkov@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/task/tasks.xlsx
+++ b/docs/task/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Number</t>
   </si>
@@ -154,6 +154,32 @@
   </si>
   <si>
     <t>Статьи править и просматривать может только мастер. Админ может только просматривать.</t>
+  </si>
+  <si>
+    <t>Реализовать добавление чемпионатов в определенную лигу. Редатирование, удаление.</t>
+  </si>
+  <si>
+    <t>ChampionshipController
+Add
+Edit</t>
+  </si>
+  <si>
+    <t>Реализовать добавление игр на сайт</t>
+  </si>
+  <si>
+    <t>GameController
+Add
+Edit
+Delete</t>
+  </si>
+  <si>
+    <t>Реализовать добавление модов на сайт</t>
+  </si>
+  <si>
+    <t>GameModController
+Add
+Edit
+Delete</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1131,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,39 +1350,63 @@
       <c r="D11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>7</v>
+      <c r="E11" s="26" t="s">
+        <v>23</v>
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+      <c r="B12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>7</v>
+      </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
+      <c r="B13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>7</v>
+      </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="B14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>7</v>
+      </c>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Some little changes for article and game controllers. Signed-off-by:Igor Peshkov <igor.peshkov@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/task/tasks.xlsx
+++ b/docs/task/tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Number</t>
   </si>
@@ -180,6 +180,12 @@
 Add
 Edit
 Delete</t>
+  </si>
+  <si>
+    <t>На главную страницу следует выводить 10 последних добавленных новостей, а не все сразу.</t>
+  </si>
+  <si>
+    <t>undex/index</t>
   </si>
 </sst>
 </file>
@@ -425,7 +431,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -473,9 +479,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1130,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1171,13 +1174,13 @@
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1191,13 +1194,13 @@
       <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="4"/>
@@ -1209,13 +1212,13 @@
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="4"/>
@@ -1227,13 +1230,13 @@
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="25" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -1247,13 +1250,13 @@
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4"/>
@@ -1265,16 +1268,16 @@
       <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="28" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1285,13 +1288,13 @@
       <c r="B8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="25" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1306,13 +1309,13 @@
       <c r="B9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1326,13 +1329,13 @@
       <c r="B10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="26" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="4"/>
@@ -1344,13 +1347,13 @@
       <c r="B11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="24" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="25" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="4"/>
@@ -1362,13 +1365,13 @@
       <c r="B12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>45</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="26" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="4"/>
@@ -1380,13 +1383,13 @@
       <c r="B13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="24" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="26" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="4"/>
@@ -1398,13 +1401,13 @@
       <c r="B14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="26" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="4"/>
@@ -1414,7 +1417,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="24"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="4"/>
@@ -1424,7 +1427,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="24"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="4"/>
@@ -1434,7 +1437,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="24"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="4"/>
@@ -1444,7 +1447,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="24"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="4"/>
@@ -1454,7 +1457,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="24"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="4"/>
@@ -1464,7 +1467,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="24"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="4"/>
@@ -1474,7 +1477,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="24"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="4"/>
@@ -1484,7 +1487,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="24"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="4"/>
@@ -1494,7 +1497,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="24"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="4"/>
@@ -1504,7 +1507,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="24"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="4"/>
@@ -1514,7 +1517,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="24"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="4"/>
@@ -1524,7 +1527,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="24"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="4"/>
@@ -1534,7 +1537,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="C27" s="24"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="4"/>
@@ -1544,7 +1547,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4"/>
-      <c r="C28" s="24"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="4"/>
@@ -1554,7 +1557,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="C29" s="24"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="4"/>
@@ -1564,7 +1567,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="24"/>
+      <c r="C30" s="23"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="4"/>
@@ -1574,7 +1577,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="24"/>
+      <c r="C31" s="23"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="4"/>
@@ -1584,7 +1587,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="24"/>
+      <c r="C32" s="23"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="4"/>
@@ -1594,7 +1597,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4"/>
-      <c r="C33" s="24"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="4"/>
@@ -1604,7 +1607,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4"/>
-      <c r="C34" s="24"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="4"/>
@@ -1614,7 +1617,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4"/>
-      <c r="C35" s="24"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="4"/>
@@ -1624,7 +1627,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4"/>
-      <c r="C36" s="24"/>
+      <c r="C36" s="23"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="4"/>
@@ -1634,7 +1637,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4"/>
-      <c r="C37" s="24"/>
+      <c r="C37" s="23"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="4"/>
@@ -1644,7 +1647,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4"/>
-      <c r="C38" s="24"/>
+      <c r="C38" s="23"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="4"/>
@@ -1654,7 +1657,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4"/>
-      <c r="C39" s="24"/>
+      <c r="C39" s="23"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="4"/>
@@ -1664,7 +1667,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4"/>
-      <c r="C40" s="24"/>
+      <c r="C40" s="23"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="4"/>
@@ -1674,7 +1677,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4"/>
-      <c r="C41" s="24"/>
+      <c r="C41" s="23"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="4"/>
@@ -1684,7 +1687,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="4"/>
-      <c r="C42" s="24"/>
+      <c r="C42" s="23"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="4"/>
@@ -1694,7 +1697,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="4"/>
-      <c r="C43" s="24"/>
+      <c r="C43" s="23"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="4"/>
@@ -1704,7 +1707,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4"/>
-      <c r="C44" s="24"/>
+      <c r="C44" s="23"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="4"/>
@@ -1714,7 +1717,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="4"/>
-      <c r="C45" s="24"/>
+      <c r="C45" s="23"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="4"/>
@@ -1724,7 +1727,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="4"/>
-      <c r="C46" s="24"/>
+      <c r="C46" s="23"/>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="4"/>
@@ -1734,7 +1737,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4"/>
-      <c r="C47" s="24"/>
+      <c r="C47" s="23"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="4"/>
@@ -1744,7 +1747,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="4"/>
-      <c r="C48" s="24"/>
+      <c r="C48" s="23"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="4"/>
@@ -1754,7 +1757,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="4"/>
-      <c r="C49" s="24"/>
+      <c r="C49" s="23"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="4"/>
@@ -1764,7 +1767,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="4"/>
-      <c r="C50" s="24"/>
+      <c r="C50" s="23"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="4"/>
@@ -1774,7 +1777,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="4"/>
-      <c r="C51" s="24"/>
+      <c r="C51" s="23"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="4"/>
@@ -1784,7 +1787,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="4"/>
-      <c r="C52" s="24"/>
+      <c r="C52" s="23"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="4"/>
@@ -1794,7 +1797,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="4"/>
-      <c r="C53" s="24"/>
+      <c r="C53" s="23"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="4"/>
@@ -1804,7 +1807,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="4"/>
-      <c r="C54" s="24"/>
+      <c r="C54" s="23"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="4"/>
@@ -1814,7 +1817,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="4"/>
-      <c r="C55" s="24"/>
+      <c r="C55" s="23"/>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="4"/>
@@ -1824,7 +1827,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="4"/>
-      <c r="C56" s="24"/>
+      <c r="C56" s="23"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="4"/>
@@ -1834,7 +1837,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="4"/>
-      <c r="C57" s="24"/>
+      <c r="C57" s="23"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="4"/>
@@ -1844,7 +1847,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="4"/>
-      <c r="C58" s="24"/>
+      <c r="C58" s="23"/>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="4"/>
@@ -1862,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1896,7 +1899,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1908,23 +1911,31 @@
       <c r="D2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="29" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="19"/>
+      <c r="B3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="20">
         <v>3</v>
       </c>
       <c r="B4" s="5"/>
@@ -1934,7 +1945,7 @@
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
       <c r="B5" s="8"/>
@@ -1944,7 +1955,7 @@
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+      <c r="A6" s="20">
         <v>5</v>
       </c>
       <c r="B6" s="5"/>
@@ -1954,7 +1965,7 @@
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>6</v>
       </c>
       <c r="B7" s="8"/>
@@ -1964,13 +1975,13 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="22">
         <v>7</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="16"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change styles and structures for championship drivres. And add breadscrumb. Fix bugs.
</commit_message>
<xml_diff>
--- a/docs/task/tasks.xlsx
+++ b/docs/task/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Number</t>
   </si>
@@ -186,13 +186,16 @@
   </si>
   <si>
     <t>undex/index</t>
+  </si>
+  <si>
+    <t>Сделать проверку для команд и гонщиков на соответствие выбранной лиге.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,15 +215,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -261,6 +255,19 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -427,11 +434,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -478,9 +485,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -493,33 +497,45 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="19">
     <dxf>
@@ -845,9 +861,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -885,7 +901,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -957,7 +973,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1174,13 +1190,13 @@
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1194,13 +1210,13 @@
       <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="4"/>
@@ -1212,13 +1228,13 @@
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="4"/>
@@ -1230,13 +1246,13 @@
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -1250,13 +1266,13 @@
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4"/>
@@ -1268,16 +1284,16 @@
       <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="27" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1288,13 +1304,13 @@
       <c r="B8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1309,13 +1325,13 @@
       <c r="B9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="22" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1329,13 +1345,13 @@
       <c r="B10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="4"/>
@@ -1347,13 +1363,13 @@
       <c r="B11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="24" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="4"/>
@@ -1365,13 +1381,13 @@
       <c r="B12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="4"/>
@@ -1383,13 +1399,13 @@
       <c r="B13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="4"/>
@@ -1401,13 +1417,13 @@
       <c r="B14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="4"/>
@@ -1417,7 +1433,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="23"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="4"/>
@@ -1427,7 +1443,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="23"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="4"/>
@@ -1437,7 +1453,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="23"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="4"/>
@@ -1447,7 +1463,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="23"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="4"/>
@@ -1457,7 +1473,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="23"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="4"/>
@@ -1467,7 +1483,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="23"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="4"/>
@@ -1477,7 +1493,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="23"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="4"/>
@@ -1487,7 +1503,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="23"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="4"/>
@@ -1497,7 +1513,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="23"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="4"/>
@@ -1507,7 +1523,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="23"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="4"/>
@@ -1517,7 +1533,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="23"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="4"/>
@@ -1527,7 +1543,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="23"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="4"/>
@@ -1537,7 +1553,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4"/>
-      <c r="C27" s="23"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="4"/>
@@ -1547,7 +1563,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4"/>
-      <c r="C28" s="23"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="4"/>
@@ -1557,7 +1573,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="C29" s="23"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="4"/>
@@ -1567,7 +1583,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="23"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="4"/>
@@ -1577,7 +1593,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="23"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="4"/>
@@ -1587,7 +1603,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="23"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="4"/>
@@ -1597,7 +1613,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4"/>
-      <c r="C33" s="23"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="4"/>
@@ -1607,7 +1623,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4"/>
-      <c r="C34" s="23"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="4"/>
@@ -1617,7 +1633,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4"/>
-      <c r="C35" s="23"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="4"/>
@@ -1627,7 +1643,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4"/>
-      <c r="C36" s="23"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="4"/>
@@ -1637,7 +1653,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4"/>
-      <c r="C37" s="23"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="4"/>
@@ -1647,7 +1663,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4"/>
-      <c r="C38" s="23"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="4"/>
@@ -1657,7 +1673,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4"/>
-      <c r="C39" s="23"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="4"/>
@@ -1667,7 +1683,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4"/>
-      <c r="C40" s="23"/>
+      <c r="C40" s="22"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="4"/>
@@ -1677,7 +1693,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4"/>
-      <c r="C41" s="23"/>
+      <c r="C41" s="22"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="4"/>
@@ -1687,7 +1703,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="4"/>
-      <c r="C42" s="23"/>
+      <c r="C42" s="22"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="4"/>
@@ -1697,7 +1713,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="4"/>
-      <c r="C43" s="23"/>
+      <c r="C43" s="22"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="4"/>
@@ -1707,7 +1723,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4"/>
-      <c r="C44" s="23"/>
+      <c r="C44" s="22"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="4"/>
@@ -1717,7 +1733,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="4"/>
-      <c r="C45" s="23"/>
+      <c r="C45" s="22"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="4"/>
@@ -1727,7 +1743,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="4"/>
-      <c r="C46" s="23"/>
+      <c r="C46" s="22"/>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="4"/>
@@ -1737,7 +1753,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4"/>
-      <c r="C47" s="23"/>
+      <c r="C47" s="22"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="4"/>
@@ -1747,7 +1763,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="4"/>
-      <c r="C48" s="23"/>
+      <c r="C48" s="22"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="4"/>
@@ -1757,7 +1773,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="4"/>
-      <c r="C49" s="23"/>
+      <c r="C49" s="22"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="4"/>
@@ -1767,7 +1783,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="4"/>
-      <c r="C50" s="23"/>
+      <c r="C50" s="22"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="4"/>
@@ -1777,7 +1793,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="4"/>
-      <c r="C51" s="23"/>
+      <c r="C51" s="22"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="4"/>
@@ -1787,7 +1803,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="4"/>
-      <c r="C52" s="23"/>
+      <c r="C52" s="22"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="4"/>
@@ -1797,7 +1813,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="4"/>
-      <c r="C53" s="23"/>
+      <c r="C53" s="22"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="4"/>
@@ -1807,7 +1823,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="4"/>
-      <c r="C54" s="23"/>
+      <c r="C54" s="22"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="4"/>
@@ -1817,7 +1833,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="4"/>
-      <c r="C55" s="23"/>
+      <c r="C55" s="22"/>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="4"/>
@@ -1827,7 +1843,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="4"/>
-      <c r="C56" s="23"/>
+      <c r="C56" s="22"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="4"/>
@@ -1837,7 +1853,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="4"/>
-      <c r="C57" s="23"/>
+      <c r="C57" s="22"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="4"/>
@@ -1847,7 +1863,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="4"/>
-      <c r="C58" s="23"/>
+      <c r="C58" s="22"/>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="4"/>
@@ -1866,7 +1882,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,7 +1915,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1911,13 +1927,13 @@
       <c r="D2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
+      <c r="A3" s="20">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1929,33 +1945,39 @@
       <c r="D3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="18"/>
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="17"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="17"/>
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
       <c r="B6" s="5"/>
@@ -1965,7 +1987,7 @@
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="20">
         <v>6</v>
       </c>
       <c r="B7" s="8"/>
@@ -1975,19 +1997,20 @@
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="21">
         <v>7</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="16"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix bugs with login form. Update innfo for slide out tabs. Add message for developmen pages. Fix bugs with post controller pages.
</commit_message>
<xml_diff>
--- a/docs/task/tasks.xlsx
+++ b/docs/task/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>Number</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Сделать проверку для команд и гонщиков на соответствие выбранной лиге.</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>Проверить элемент checkBox для формы авторизации на главной странице</t>
   </si>
 </sst>
 </file>
@@ -438,7 +444,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -528,6 +534,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -825,6 +834,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -903,7 +915,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -938,7 +950,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1149,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,8 +1399,8 @@
       <c r="D12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>7</v>
+      <c r="E12" s="24" t="s">
+        <v>23</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -1405,8 +1417,8 @@
       <c r="D13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>7</v>
+      <c r="E13" s="26" t="s">
+        <v>53</v>
       </c>
       <c r="F13" s="4"/>
     </row>
@@ -1423,8 +1435,8 @@
       <c r="D14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>7</v>
+      <c r="E14" s="26" t="s">
+        <v>53</v>
       </c>
       <c r="F14" s="4"/>
     </row>
@@ -1882,7 +1894,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,8 +1939,8 @@
       <c r="D2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="28" t="s">
-        <v>7</v>
+      <c r="E2" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="F2" s="9"/>
     </row>
@@ -1961,19 +1973,23 @@
       <c r="D4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="28" t="s">
-        <v>7</v>
+      <c r="E4" s="32" t="s">
+        <v>23</v>
       </c>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="C5" s="30"/>
       <c r="D5" s="31"/>
-      <c r="E5" s="17"/>
+      <c r="E5" s="28" t="s">
+        <v>7</v>
+      </c>
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>